<commit_message>
adjustments in project structure and correction of own zeiterfassung
</commit_message>
<xml_diff>
--- a/documents/00_Sitzungen/Milestone_2/Zeitaufwanderfassung/Zeiterfassung_xlsx/23_Zeiterfassung MS2_Histarantia.xlsx
+++ b/documents/00_Sitzungen/Milestone_2/Zeitaufwanderfassung/Zeiterfassung_xlsx/23_Zeiterfassung MS2_Histarantia.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raphael\git\ps_17_gruppe23\documents\00_Sitzungen\Milestone_2\Zeitaufwanderfassung\Zeiterfassung_xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CF2774E-093D-4A99-8968-F37C37170B4D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4AD33DF-99A8-4D25-AD08-EDFB1732B725}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" xr2:uid="{41C5A5EF-7409-4D51-A49E-327120042783}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" calcMode="manual"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -621,7 +621,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
correction due to error in my own zeiterfassung.
</commit_message>
<xml_diff>
--- a/documents/00_Sitzungen/Milestone_2/Zeitaufwanderfassung/Zeiterfassung_xlsx/23_Zeiterfassung MS2_Histarantia.xlsx
+++ b/documents/00_Sitzungen/Milestone_2/Zeitaufwanderfassung/Zeiterfassung_xlsx/23_Zeiterfassung MS2_Histarantia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raphael\git\ps_17_gruppe23\documents\00_Sitzungen\Milestone_2\Zeitaufwanderfassung\Zeiterfassung_xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4AD33DF-99A8-4D25-AD08-EDFB1732B725}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF14A7C8-3921-45C6-9104-F6C88D1B71AB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" xr2:uid="{41C5A5EF-7409-4D51-A49E-327120042783}"/>
   </bookViews>
@@ -120,7 +120,7 @@
     <t>105.25 Stunden</t>
   </si>
   <si>
-    <t>35.25 Stunden</t>
+    <t>34.75 Stunden</t>
   </si>
 </sst>
 </file>
@@ -621,7 +621,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>